<commit_message>
fix colorful ad info error
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625EA127-73B0-458E-BA79-0AE2D04C1414}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB085896-9434-496F-BDA5-E9CDDDBDCD89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="4260" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="165">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -536,10 +536,6 @@
   </si>
   <si>
     <t>Colorful iGameRTX3090 Advanced OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPI uP9511R?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -890,6 +886,16 @@
   </si>
   <si>
     <t>vRAMController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI uP9512R?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnSemi 
+NCP302150
+(50A DrMOS)?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1273,7 +1279,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1299,7 +1305,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1308,10 +1314,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
         <v>162</v>
-      </c>
-      <c r="E1" t="s">
-        <v>163</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -1447,7 +1453,7 @@
         <v>21</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>38</v>
@@ -1462,7 +1468,7 @@
         <v>42</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
@@ -1503,7 +1509,7 @@
         <v>49</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>35</v>
@@ -1523,63 +1529,63 @@
     </row>
     <row r="5" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
         <v>108</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>90</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>42</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
@@ -1600,10 +1606,10 @@
         <v>30</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>50</v>
@@ -1830,22 +1836,22 @@
         <v>89</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>82</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>94</v>
@@ -1862,28 +1868,28 @@
         <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="G11" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>47</v>
@@ -1892,25 +1898,25 @@
         <v>16</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="P11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>95</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1933,7 +1939,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1959,7 +1965,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1968,10 +1974,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
         <v>162</v>
-      </c>
-      <c r="E1" t="s">
-        <v>163</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -2015,114 +2021,114 @@
     </row>
     <row r="2" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
-        <v>109</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="K2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>42</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>95</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -2130,60 +2136,60 @@
         <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="P4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>95</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
@@ -2204,22 +2210,22 @@
         <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>56</v>
@@ -2234,7 +2240,7 @@
         <v>95</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -2320,7 +2326,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R11" s="3"/>
     </row>

</xml_diff>

<commit_message>
add Gigabyte RTX3080 Gaming OC
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DCCFF5-EB96-4BD9-91A6-C293A54BACC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF4CCED-D7E9-429F-AF80-77E0C5AFC67A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="4260" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <author>william</author>
   </authors>
   <commentList>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{FBAA4AB8-5643-46E0-B9F5-61A049D7FD79}">
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{FBAA4AB8-5643-46E0-B9F5-61A049D7FD79}">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="196">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -158,10 +158,6 @@
   </si>
   <si>
     <t>Gigabyte GeForce RTX 3090 Gaming OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>370/390W</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -552,13 +548,6 @@
   <si>
     <t>expreview.com/76297.html
 3c.3dmgame.com/show-16-13206-1.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>65°C/1824rpm
-（expreview)
-65°C/1826rpm
-（3dmgame)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1016,6 +1005,63 @@
   <si>
     <t>138
 mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gigabyte GeForce RTX 3080 Gaming OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13-phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS AOZ5332QI
+（50A DrMOS）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">370/390W
+(OC BIOS)
+350W/350w
+(SILENT BIOS)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">375/375W
+(OC BIOS)
+345/345W
+(SILENT BIOS)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2*9cm+1*8cm
+2600rpm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1800/
+?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65°C/1824rpm
+（expreview,27℃)
+65°C/1826rpm
+（3dmgame)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65°C/1807rpm
+70°C/1507rpm
+（expreview,25°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76104.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1407,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1434,7 +1480,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1443,10 +1489,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -1470,19 +1516,19 @@
         <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
-        <v>34</v>
-      </c>
       <c r="Q1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
@@ -1490,58 +1536,58 @@
     </row>
     <row r="2" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>181</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -1552,10 +1598,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -1570,10 +1616,10 @@
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>17</v>
@@ -1582,25 +1628,25 @@
         <v>18</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="4" spans="1:18" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1608,10 +1654,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -1626,219 +1672,219 @@
         <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>101</v>
+        <v>193</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="Q5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
         <v>106</v>
       </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="E6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="Q6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
@@ -1847,54 +1893,54 @@
         <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>9</v>
@@ -1903,54 +1949,54 @@
         <v>11</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R9" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
@@ -1959,149 +2005,149 @@
         <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" t="s">
-        <v>162</v>
-      </c>
-      <c r="E12" t="s">
-        <v>162</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -2121,10 +2167,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2150,7 +2196,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2159,10 +2205,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -2186,19 +2232,19 @@
         <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
-        <v>34</v>
-      </c>
       <c r="Q1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
@@ -2206,300 +2252,342 @@
     </row>
     <row r="2" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
         <v>164</v>
-      </c>
-      <c r="B2" t="s">
-        <v>166</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>177</v>
-      </c>
     </row>
-    <row r="3" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>107</v>
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="O4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="114" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="L5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="K6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" ht="114" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N4" s="1" t="s">
+    <row r="7" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="57" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="Q7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D8" s="1"/>
       <c r="F8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2525,7 +2613,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="3"/>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F10" s="1"/>
@@ -2553,7 +2641,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="2"/>
+      <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F12" s="1"/>
@@ -2566,13 +2654,27 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="R12" s="3"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
       <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M14" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add ZOTAC RTX 3080 Apocalypse OC
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF4CCED-D7E9-429F-AF80-77E0C5AFC67A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D058FF3D-2514-41B1-B906-224A4EA64215}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="5325" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="205">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -403,13 +403,6 @@
     <t>1395/
 1710/
 1965?MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74°C/1800rpm
-（expreview)
-74°C/?rpm
-（pconline)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1062,6 +1055,55 @@
   </si>
   <si>
     <t>www.expreview.com/76104.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZOTAC RTX 3080 Apocalypse OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2*9cm+1*8cm
+?rpm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74°C/1800rpm
+（expreview,27°C)
+74°C/?rpm
+（pconline)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72°C/?rpm
+（expreview,25°)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320W/?W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI us5650P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1710/
+?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>315
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>122
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76430.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1453,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1480,7 +1522,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1489,10 +1531,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" t="s">
         <v>158</v>
-      </c>
-      <c r="E1" t="s">
-        <v>159</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -1536,49 +1578,49 @@
     </row>
     <row r="2" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" t="s">
-        <v>163</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>39</v>
@@ -1587,7 +1629,7 @@
         <v>41</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -1601,7 +1643,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -1616,7 +1658,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>45</v>
@@ -1657,7 +1699,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -1672,7 +1714,7 @@
         <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>46</v>
@@ -1681,10 +1723,10 @@
         <v>17</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>37</v>
@@ -1699,7 +1741,7 @@
         <v>41</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
@@ -1740,7 +1782,7 @@
         <v>48</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>34</v>
@@ -1760,63 +1802,63 @@
     </row>
     <row r="6" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
       </c>
       <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
         <v>105</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -1825,7 +1867,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -1837,10 +1879,10 @@
         <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>49</v>
@@ -1864,7 +1906,7 @@
         <v>56</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>57</v>
@@ -1884,7 +1926,7 @@
         <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
@@ -1896,7 +1938,7 @@
         <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>66</v>
@@ -1920,7 +1962,7 @@
         <v>36</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>64</v>
@@ -1940,7 +1982,7 @@
         <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>9</v>
@@ -1964,7 +2006,7 @@
         <v>65</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>72</v>
+        <v>197</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>37</v>
@@ -1976,15 +2018,15 @@
         <v>70</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -2005,45 +2047,45 @@
         <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
@@ -2061,66 +2103,66 @@
         <v>29</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="E12" t="s">
-        <v>160</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="G12" t="s">
         <v>29</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>46</v>
@@ -2129,25 +2171,25 @@
         <v>16</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="P12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -2170,7 +2212,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2196,7 +2238,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2205,10 +2247,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" t="s">
         <v>158</v>
-      </c>
-      <c r="E1" t="s">
-        <v>159</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -2252,78 +2294,78 @@
     </row>
     <row r="2" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G2" t="s">
-        <v>163</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
         <v>186</v>
-      </c>
-      <c r="B3" t="s">
-        <v>187</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
@@ -2332,19 +2374,19 @@
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>37</v>
@@ -2359,136 +2401,136 @@
         <v>41</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" t="s">
         <v>105</v>
       </c>
-      <c r="E4" t="s">
-        <v>106</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G5" t="s">
         <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="Q5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>52</v>
@@ -2497,42 +2539,42 @@
         <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
         <v>59</v>
@@ -2541,7 +2583,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -2553,22 +2595,22 @@
         <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>55</v>
@@ -2580,26 +2622,67 @@
         <v>56</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2"/>
+    <row r="8" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F9" s="1"/>
@@ -2669,7 +2752,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R13" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix many PWM controller model errors
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D058FF3D-2514-41B1-B906-224A4EA64215}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB89D080-D604-453A-8101-F3C0CC3053F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="6390" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="203">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,10 +92,6 @@
   </si>
   <si>
     <t>3-phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPI uS5650Q</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -457,17 +453,6 @@
   <si>
     <t>135
 mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPI uP9511R+
-UPI uP9512R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnSemi 
-NCP81611+
-UPI uP9512R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -889,12 +874,6 @@
   </si>
   <si>
     <t>MPS
-MP2884B+
-MP2888B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MPS
 MP86957
 (70A DrMOS)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -962,20 +941,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MPS
-MP2884B+
-MP2886B+
-MP2888B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">11cm+11cm
 3600rpm?
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPI uS5650Q?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1083,10 +1051,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UPI us5650P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1440/
 1710/
 ?MHZ</t>
@@ -1104,6 +1068,32 @@
   </si>
   <si>
     <t>www.expreview.com/76430.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPS
+MP2884B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPS
+MP2886B+
+MP2888B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASUS TUF GeForce RTX 3080 Gaming OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnSemi 
+NCP81611</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI 
+uP9511R+
+uP9512R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1495,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1522,7 +1512,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1531,105 +1521,105 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
-        <v>33</v>
-      </c>
       <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="57" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="G2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -1640,556 +1630,556 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
+        <v>202</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="M3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="I5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="M6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="Q6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
+        <v>101</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R9" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="K10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R10" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="R11" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -2212,7 +2202,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2238,7 +2228,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2247,441 +2237,441 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
-        <v>33</v>
-      </c>
       <c r="Q1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="G2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="N3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="P4" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="B5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="O6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
+        <v>101</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="P8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -2752,7 +2742,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="R13" s="3"/>
     </row>

</xml_diff>

<commit_message>
Correctly distinguish the difference between ASUS TUF Gaming OC and ASUS TUF Gaming
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB89D080-D604-453A-8101-F3C0CC3053F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54BD3EF-3700-44FC-BA85-41DE95C6574F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="7455" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <author>william</author>
   </authors>
   <commentList>
-    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{724FB272-25E8-49C8-A960-99B0C1CBFF64}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{724FB272-25E8-49C8-A960-99B0C1CBFF64}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
     <author>william</author>
   </authors>
   <commentList>
-    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{FBAA4AB8-5643-46E0-B9F5-61A049D7FD79}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{FBAA4AB8-5643-46E0-B9F5-61A049D7FD79}">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="212">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -648,17 +648,6 @@
     <t>65°C/1857rpm
 71°C/1606rpm
 （techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>63°C/2014rpm
-71°C/1862rpm
-（techpowerup)
-62°C/1900rpm
-66°C/1500rpm
-（chiphell,21°C)
-61°C/1800rpm
-（koolshare)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -753,12 +742,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>www.techpowerup.com/review/asus-geforce-rtx-3080-tuf-gaming-oc/
-www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=4
-koolshare.cn/thread-187771-1-1.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1094,6 +1077,63 @@
     <t>UPI 
 uP9511R+
 uP9512R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASUS TUF GeForce RTX 3080 Gaming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VISHAY
+SIC651A?
+(55A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1710/
+1960?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?/?W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">63°C/2014rpm
+71°C/1862rpm
+（techpowerup)
+62°C/1900rpm
+66°C/1500rpm
+（chiphell,21°C)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">www.techpowerup.com/review/asus-geforce-rtx-3080-tuf-gaming-oc/
+www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=4
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>koolshare.cn/thread-187771-1-1.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+61°C/1800rpm
+（koolshare,27°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>350/375W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>news.mydrivers.com/1/716/716139.htm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1483,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1512,7 +1552,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1521,10 +1561,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1568,7 +1608,7 @@
     </row>
     <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
         <v>100</v>
@@ -1577,25 +1617,25 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
@@ -1604,13 +1644,13 @@
         <v>109</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>38</v>
@@ -1619,7 +1659,7 @@
         <v>40</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -1633,7 +1673,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>101</v>
@@ -1689,7 +1729,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>101</v>
@@ -1713,10 +1753,10 @@
         <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>36</v>
@@ -1807,7 +1847,7 @@
         <v>102</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>10</v>
@@ -1825,10 +1865,10 @@
         <v>16</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>109</v>
+        <v>209</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>116</v>
+        <v>210</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>110</v>
@@ -1843,68 +1883,68 @@
         <v>40</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>107</v>
+        <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>201</v>
+      <c r="E7" t="s">
+        <v>102</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
+        <v>103</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
@@ -1912,55 +1952,55 @@
       <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>59</v>
+      <c r="D8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
@@ -1984,10 +2024,10 @@
         <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>15</v>
@@ -1996,27 +2036,27 @@
         <v>64</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>191</v>
+        <v>61</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R9" s="3" t="s">
-        <v>71</v>
+      <c r="R9" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -2037,45 +2077,45 @@
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>86</v>
+        <v>189</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -2090,100 +2130,156 @@
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>79</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>91</v>
+      <c r="R11" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="114" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R12" s="3" t="s">
+      <c r="R12" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="114" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="M13" s="1"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M14" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2199,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2228,7 +2324,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2237,10 +2333,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -2284,66 +2380,66 @@
     </row>
     <row r="2" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
         <v>158</v>
-      </c>
-      <c r="B2" t="s">
-        <v>160</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -2355,7 +2451,7 @@
         <v>101</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -2364,19 +2460,19 @@
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>36</v>
@@ -2391,12 +2487,12 @@
         <v>40</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
         <v>100</v>
@@ -2411,7 +2507,7 @@
         <v>102</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>10</v>
@@ -2420,7 +2516,7 @@
         <v>108</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>117</v>
@@ -2432,7 +2528,7 @@
         <v>114</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>120</v>
+        <v>205</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>110</v>
@@ -2447,136 +2543,136 @@
         <v>40</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>137</v>
+        <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="114" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
         <v>102</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
+        <v>121</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>132</v>
+        <v>203</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>133</v>
+        <v>208</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>126</v>
+        <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>51</v>
+        <v>130</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R6" s="2" t="s">
-        <v>138</v>
+      <c r="R6" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>201</v>
+      <c r="E7" t="s">
+        <v>101</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>51</v>
@@ -2585,108 +2681,150 @@
         <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R7" s="3" t="s">
-        <v>145</v>
+      <c r="R7" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>59</v>
+      <c r="D8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>181</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>139</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>113</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>195</v>
+        <v>54</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>196</v>
+        <v>34</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>197</v>
+      <c r="R8" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="F9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="2"/>
+    <row r="9" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F10" s="1"/>
@@ -2700,7 +2838,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="3"/>
+      <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>
@@ -2728,7 +2866,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="2"/>
+      <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F13" s="1"/>
@@ -2741,13 +2879,27 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="R13" s="3"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
       <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add colorful rtx3080 vulcan expreview test data
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEFBCFE-A8CC-4E38-BE54-DACAB2B59B4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85FE301-5345-4267-8EED-F5B72EBB37FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9585" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="10650" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -25,54 +25,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>william</author>
-  </authors>
-  <commentList>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{724FB272-25E8-49C8-A960-99B0C1CBFF64}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Some sources report that MSI has recently cancelled the heat pipe direct contact design.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>william</author>
-  </authors>
-  <commentList>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{FBAA4AB8-5643-46E0-B9F5-61A049D7FD79}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Some sources report that MSI has recently cancelled the heat pipe direct contact design.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="225">
   <si>
@@ -506,10 +458,6 @@
   </si>
   <si>
     <t>www.techpowerup.com/review/evga-geforce-rtx-3090-ftw3-ultra/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Colorful iGameRTX3090 Advanced OC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -673,12 +621,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">diy.zol.com.cn/752/7524846.html
-www.techpowerup.com/review/colorful-igame-geforce-rtx-3080-vulcan-oc/
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>158.5
 mm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -710,6 +652,477 @@
     <t>1440/
 1800/
 1980MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>67°C/2260rpm
+（chiphell,21°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320/340W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74°C/?rpm
+（pconline)
+65°C/1953rpm
+(3dmgame,normal)
+65°C/1783rpm
+(3dmgame,Turbo BIOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1710/
+2040MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-phase6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6*6mm + 1*8mm 
+heat pipes with direct touching
+non-metal backplate with 2 heat pipes and thermal pads(*)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>340/350W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSI GeForce RTX 3080 Gaming X Trio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSI GeForce RTX 3090 Gaming X Trio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.techpowerup.com/review/msi-geforce-rtx-3080-gaming-x-trio/
+www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*9cm
+3200rpm?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1710/
+2055MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64°C/2030rpm
+（chiphell,21°C)
+65°C/1838rpm
+76°C/1500rpm
+（techpowerup)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6*6mm + 1*8mm 
+heat pipes with direct touching
+metal backplate with 2 heat pipes and thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>420W/450W
+420W/500W
+(XOC BIOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>350/?W
+370/?W
+(Turbo BIOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320/340W
+370/400W
+(Turbo BIOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vGPUController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vRAMController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI uP9512R?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnSemi 
+NCP302150
+(50A DrMOS)?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVIDIA Geforce RTX3080 Founders Edition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1*12PIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15-phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPS
+MP86957
+(70A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>285
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>112
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"2-slot"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4*8mm heat pipe with vapor chamber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1770/
+2010MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320/370W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">8cm+8cm?
+3600rpm?
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*9cm
+2500rpm?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.techpowerup.com/review/nvidia-geforce-rtx-3080-founders-edition/
+www.expreview.com/75997.html
+diy.pconline.com.cn/1370/13708125_all.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>78°C/19770rpm
+（techpowerup)
+77°C/?rpm
+（expreview,26°C)
+78°C/?rpm
+(pconline)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVIDIA Geforce RTX3090 Founders Edition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76296.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">11cm+11cm
+3600rpm?
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+71°C/2600rpm
+（expreview,28°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1395/
+1695/
+1860MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>313
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>138
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gigabyte GeForce RTX 3080 Gaming OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13-phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS AOZ5332QI
+（50A DrMOS）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">370/390W
+(OC BIOS)
+350W/350w
+(SILENT BIOS)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">375/375W
+(OC BIOS)
+345/345W
+(SILENT BIOS)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2*9cm+1*8cm
+2600rpm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1800/
+?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65°C/1824rpm
+（expreview,27℃)
+65°C/1826rpm
+（3dmgame)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65°C/1807rpm
+70°C/1507rpm
+（expreview,25°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76104.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2*9cm+1*8cm
+?rpm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74°C/1800rpm
+（expreview,27°C)
+74°C/?rpm
+（pconline)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72°C/?rpm
+（expreview,25°)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1710/
+?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>315
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>122
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76430.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPS
+MP2884B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPS
+MP2886B+
+MP2888B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASUS TUF GeForce RTX 3080 Gaming OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnSemi 
+NCP81611</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI 
+uP9511R+
+uP9512R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASUS TUF GeForce RTX 3080 Gaming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VISHAY
+SIC651A?
+(55A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1710/
+1960?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?/?W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">63°C/2014rpm
+71°C/1862rpm
+（techpowerup)
+62°C/1900rpm
+66°C/1500rpm
+（chiphell,21°C)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">www.techpowerup.com/review/asus-geforce-rtx-3080-tuf-gaming-oc/
+www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=4
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>koolshare.cn/thread-187771-1-1.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+61°C/1800rpm
+（koolshare,27°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>news.xfastest.com/review/review-05/85808/asus-tuf-gaming-rtx-3090/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320/?W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320/320W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76107.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS
+AOZ5311QI
+（50A DrMOS）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6*6mm heat pipes with nickel-plated copper base plate
+metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1710/
+1890?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73°C/?rpm
+（expreview,27°)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>332
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>129
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6*6mm heat pipes with copper base plate
+metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72°C/1940rpm
+（chiphell,21°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">diy.zol.com.cn/752/7524846.html
+www.techpowerup.com/review/colorful-igame-geforce-rtx-3080-vulcan-oc/
+www.expreview.com/76519.html
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -720,483 +1133,25 @@
 (normal)
 72°C/1912rpm
 (Turbo BIOS)
-(techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>67°C/2260rpm
-（chiphell,21°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>320/340W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74°C/?rpm
-（pconline)
-65°C/1953rpm
-(3dmgame,normal)
-65°C/1783rpm
-(3dmgame,Turbo BIOS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1440/
-1710/
-2040MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-phase6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6*6mm + 1*8mm 
-heat pipes with direct touching
-non-metal backplate with 2 heat pipes and thermal pads(*)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>340/350W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSI GeForce RTX 3080 Gaming X Trio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSI GeForce RTX 3090 Gaming X Trio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.techpowerup.com/review/msi-geforce-rtx-3080-gaming-x-trio/
-www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3*9cm
-3200rpm?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1440/
-1710/
-2055MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>64°C/2030rpm
-（chiphell,21°C)
-65°C/1838rpm
-76°C/1500rpm
-（techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6*6mm + 1*8mm 
-heat pipes with direct touching
-metal backplate with 2 heat pipes and thermal pads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>420W/450W
-420W/500W
-(XOC BIOS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>350/?W
-370/?W
-(Turbo BIOS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>320/340W
-370/400W
-(Turbo BIOS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vGPUController</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vRAMController</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPI uP9512R?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnSemi 
-NCP302150
-(50A DrMOS)?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NVIDIA Geforce RTX3080 Founders Edition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1*12PIN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>15-phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MPS
-MP86957
-(70A DrMOS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>285
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>112
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"2-slot"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4*8mm heat pipe with vapor chamber</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1440/
-1770/
-2010MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>320/370W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">8cm+8cm?
-3600rpm?
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3*9cm
-2500rpm?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.techpowerup.com/review/nvidia-geforce-rtx-3080-founders-edition/
-www.expreview.com/75997.html
-diy.pconline.com.cn/1370/13708125_all.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>78°C/19770rpm
-（techpowerup)
-77°C/?rpm
-（expreview,26°C)
-78°C/?rpm
-(pconline)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NVIDIA Geforce RTX3090 Founders Edition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.expreview.com/76296.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">11cm+11cm
-3600rpm?
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">
-71°C/2600rpm
-（expreview,28°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1395/
-1695/
-1860MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>313
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>138
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gigabyte GeForce RTX 3080 Gaming OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13-phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS AOZ5332QI
-（50A DrMOS）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">370/390W
-(OC BIOS)
-350W/350w
-(SILENT BIOS)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">375/375W
-(OC BIOS)
-345/345W
-(SILENT BIOS)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2*9cm+1*8cm
-2600rpm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1440/
-1800/
-?MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>65°C/1824rpm
-（expreview,27℃)
-65°C/1826rpm
-（3dmgame)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>65°C/1807rpm
-70°C/1507rpm
+(techpowerup)
+67°C/1725rpm
 （expreview,25°C)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>www.expreview.com/76104.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZOTAC RTX 3080 Apocalypse OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2*9cm+1*8cm
-?rpm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74°C/1800rpm
-（expreview,27°C)
-74°C/?rpm
-（pconline)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>72°C/?rpm
-（expreview,25°)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1440/
-1710/
-?MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>315
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>122
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.expreview.com/76430.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MPS
-MP2884B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MPS
-MP2886B+
-MP2888B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASUS TUF GeForce RTX 3080 Gaming OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnSemi 
-NCP81611</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPI 
-uP9511R+
-uP9512R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASUS TUF GeForce RTX 3080 Gaming</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VISHAY
-SIC651A?
-(55A DrMOS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1440/
-1710/
-1960?MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?/?W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">63°C/2014rpm
-71°C/1862rpm
-（techpowerup)
-62°C/1900rpm
-66°C/1500rpm
-（chiphell,21°C)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">www.techpowerup.com/review/asus-geforce-rtx-3080-tuf-gaming-oc/
-www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=4
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>koolshare.cn/thread-187771-1-1.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-61°C/1800rpm
-（koolshare,27°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>news.xfastest.com/review/review-05/85808/asus-tuf-gaming-rtx-3090/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>320/?W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>320/320W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.expreview.com/76107.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS
-AOZ5311QI
-（50A DrMOS）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6*6mm heat pipes with nickel-plated copper base plate
-metal backplate with thermal pads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1440/
-1710/
-1890?MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73°C/?rpm
-（expreview,27°)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>332
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>129
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>64
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6*6mm heat pipes with copper base plate
-metal backplate with thermal pads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>72°C/1940rpm
-（chiphell,21°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GALAX RTX 3080 Black General</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GALAX RTX 3080 Metal Master</t>
+    <t>Colorful iGame GeForce RTX3090 Advanced OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZOTAC GeForce RTX 3080 Apocalypse OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GALAX GeForce RTX 3080 Black General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GALAX GeForce RTX 3080 Metal Master</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1204,7 +1159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1219,13 +1174,6 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1269,7 +1217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1585,16 +1533,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.625" customWidth="1"/>
+    <col min="1" max="1" width="40.625" customWidth="1"/>
     <col min="2" max="2" width="10.25" customWidth="1"/>
     <col min="3" max="3" width="9.75" customWidth="1"/>
     <col min="4" max="4" width="12.875" customWidth="1"/>
@@ -1615,7 +1563,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1624,10 +1572,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1671,49 +1619,49 @@
     </row>
     <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>38</v>
@@ -1722,7 +1670,7 @@
         <v>40</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -1736,10 +1684,10 @@
         <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -1792,10 +1740,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
@@ -1816,10 +1764,10 @@
         <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>36</v>
@@ -1834,7 +1782,7 @@
         <v>40</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
@@ -1875,7 +1823,7 @@
         <v>47</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>33</v>
@@ -1895,119 +1843,119 @@
     </row>
     <row r="6" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" t="s">
         <v>101</v>
       </c>
-      <c r="E6" t="s">
-        <v>102</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>85</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
         <v>101</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>85</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
@@ -2016,10 +1964,10 @@
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>51</v>
@@ -2028,10 +1976,10 @@
         <v>28</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>48</v>
@@ -2155,7 +2103,7 @@
         <v>64</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>36</v>
@@ -2258,22 +2206,22 @@
         <v>84</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>79</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>89</v>
@@ -2287,31 +2235,31 @@
     </row>
     <row r="13" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>221</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>45</v>
@@ -2320,25 +2268,25 @@
         <v>15</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="P13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -2348,7 +2296,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <webPublishItems count="2">
     <webPublishItem id="28498" divId="GraphicsCardSpecificationTable_28498" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\GraphicsCardSpecificationTable.htm"/>
     <webPublishItem id="5606" divId="GraphicsCardSpecificationTable_5606" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\Page.html"/>
@@ -2357,16 +2304,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.625" customWidth="1"/>
+    <col min="1" max="1" width="40.625" customWidth="1"/>
     <col min="2" max="2" width="10.25" customWidth="1"/>
     <col min="3" max="3" width="9.75" customWidth="1"/>
     <col min="4" max="4" width="12.875" customWidth="1"/>
@@ -2387,7 +2334,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2396,10 +2343,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -2443,78 +2390,78 @@
     </row>
     <row r="2" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="G2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -2523,19 +2470,19 @@
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>36</v>
@@ -2550,192 +2497,192 @@
         <v>40</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
         <v>101</v>
       </c>
-      <c r="E4" t="s">
-        <v>102</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
         <v>101</v>
       </c>
-      <c r="E5" t="s">
-        <v>102</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="N5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="114" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>132</v>
+        <v>220</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>125</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>221</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>51</v>
@@ -2744,42 +2691,42 @@
         <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="N7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="P7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
         <v>58</v>
@@ -2788,10 +2735,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>51</v>
@@ -2800,22 +2747,22 @@
         <v>28</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>54</v>
@@ -2830,15 +2777,15 @@
         <v>90</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -2850,7 +2797,7 @@
         <v>59</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
@@ -2859,25 +2806,25 @@
         <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="O9" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>69</v>
@@ -2886,7 +2833,7 @@
         <v>90</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
@@ -2906,43 +2853,43 @@
         <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>52</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -2968,37 +2915,37 @@
         <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>52</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -3041,7 +2988,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R14" s="3"/>
     </row>
@@ -3052,6 +2999,5 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix rtx3080/3090 fe outputs error
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA168B86-1F86-40E2-B1C9-AE5B74838509}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2A41DA-0664-4578-A350-CB478BC77D3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="12780" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -839,15 +839,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>78°C/19770rpm
-（techpowerup)
-77°C/?rpm
-（expreview,26°C)
-78°C/?rpm
-(pconline)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NVIDIA Geforce RTX3090 Founders Edition</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1217,6 +1208,15 @@
   <si>
     <t>www.techpowerup.com/review/nvidia-geforce-rtx-3070-founders-edition/
 www.expreview.com/76296.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>78°C/1977rpm
+（techpowerup)
+77°C/?rpm
+（expreview,26°C)
+78°C/?rpm
+(pconline)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1605,7 +1605,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
         <v>99</v>
@@ -1696,10 +1696,10 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>156</v>
@@ -1711,10 +1711,10 @@
         <v>160</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
@@ -1723,22 +1723,22 @@
         <v>108</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -1752,7 +1752,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>100</v>
@@ -1808,7 +1808,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>100</v>
@@ -1832,10 +1832,10 @@
         <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>36</v>
@@ -1926,7 +1926,7 @@
         <v>101</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>10</v>
@@ -1938,16 +1938,16 @@
         <v>85</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>109</v>
@@ -1962,7 +1962,7 @@
         <v>40</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
@@ -2035,7 +2035,7 @@
         <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>51</v>
@@ -2171,7 +2171,7 @@
         <v>64</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>36</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="13" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>
@@ -2375,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2467,10 +2467,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>156</v>
@@ -2494,7 +2494,7 @@
         <v>162</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>166</v>
+        <v>237</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>157</v>
@@ -2506,7 +2506,7 @@
         <v>159</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>165</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="3" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
         <v>174</v>
-      </c>
-      <c r="B3" t="s">
-        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -2529,7 +2529,7 @@
         <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -2538,19 +2538,19 @@
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>112</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>36</v>
@@ -2565,12 +2565,12 @@
         <v>40</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
@@ -2606,7 +2606,7 @@
         <v>113</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>109</v>
@@ -2621,12 +2621,12 @@
         <v>40</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
         <v>99</v>
@@ -2653,16 +2653,16 @@
         <v>164</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>112</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>109</v>
@@ -2677,7 +2677,7 @@
         <v>40</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="142.5" x14ac:dyDescent="0.2">
@@ -2718,7 +2718,7 @@
         <v>147</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>54</v>
@@ -2733,12 +2733,12 @@
         <v>90</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
         <v>99</v>
@@ -2806,7 +2806,7 @@
         <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>51</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="9" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -2865,7 +2865,7 @@
         <v>59</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
@@ -2874,25 +2874,25 @@
         <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>112</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>69</v>
@@ -2901,12 +2901,12 @@
         <v>90</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
         <v>58</v>
@@ -2921,48 +2921,48 @@
         <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>52</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>112</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
@@ -2983,7 +2983,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>52</v>
@@ -2998,22 +2998,22 @@
         <v>131</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N11" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>90</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -3074,7 +3074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B74EFA-8FE9-4490-883F-CFD8830FE35D}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
@@ -3157,46 +3157,46 @@
     </row>
     <row r="2" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" t="s">
         <v>225</v>
-      </c>
-      <c r="C2" t="s">
-        <v>226</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G2" t="s">
         <v>154</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>158</v>
@@ -3208,7 +3208,7 @@
         <v>90</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add 3 rtx3070 cards
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2A41DA-0664-4578-A350-CB478BC77D3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F37F3CD-C21A-4C8E-B4B7-D0F55CDB2F2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="13845" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="269">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>Fans</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS AOZ5332QI+
-AOZ5311QI
-（50A DrMOS）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -111,11 +105,6 @@
   </si>
   <si>
     <t>Full Load Temp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71°C/1809rpm
-（techpowerup)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -300,17 +289,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>67°C/2016rpm
-77°C/1543rpm
-（techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>76°C/1700rpm
-（techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>120.7
 mm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -433,13 +411,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>77°C/?rpm
-（pconline)
-73°C/2137rpm
-（3dmgame)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t> EVGA GeForce RTX 3090 FTW3 Ultra</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -573,33 +544,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>68°C/2000?rpm
-（koolshare,27°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1440/
 1785/
 2025MHZ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">68°C/2175rpm
-68°C/1615rpm
-（techpowerup)
-67°C/1850rpm
-72°C/1500rpm
-（chiphell,21°C)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>65°C/1857rpm
-71°C/1606rpm
-（techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>`</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -642,35 +592,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AOS
-AOZ5311QI+
-ONSEMI
-NCP303151
-（50A DrMOS）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1440/
 1800/
 1980MHZ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>67°C/2260rpm
-（chiphell,21°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>320/340W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74°C/?rpm
-（pconline)
-65°C/1953rpm
-(3dmgame,normal)
-65°C/1783rpm
-(3dmgame,Turbo BIOS)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -722,14 +650,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>64°C/2030rpm
-（chiphell,21°C)
-65°C/1838rpm
-76°C/1500rpm
-（techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>6*6mm + 1*8mm 
 heat pipes with direct touching
 metal backplate with 2 heat pipes and thermal pads</t>
@@ -853,12 +773,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">
-71°C/2600rpm
-（expreview,28°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1395/
 1695/
 1860MHZ</t>
@@ -880,11 +794,6 @@
   </si>
   <si>
     <t>13-phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS AOZ5332QI
-（50A DrMOS）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -915,37 +824,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>65°C/1824rpm
-（expreview,27℃)
-65°C/1826rpm
-（3dmgame)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>65°C/1807rpm
-70°C/1507rpm
-（expreview,25°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>www.expreview.com/76104.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2*9cm+1*8cm
 ?rpm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74°C/1800rpm
-（expreview,27°C)
-74°C/?rpm
-（pconline)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>72°C/?rpm
-（expreview,25°)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1015,16 +899,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">63°C/2014rpm
-71°C/1862rpm
-（techpowerup)
-62°C/1900rpm
-66°C/1500rpm
-（chiphell,21°C)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">www.techpowerup.com/review/asus-geforce-rtx-3080-tuf-gaming-oc/
 www.chiphell.com/portal.php?mod=view&amp;aid=24231&amp;page=4
 </t>
@@ -1034,12 +908,6 @@
     <t>koolshare.cn/thread-187771-1-1.html</t>
   </si>
   <si>
-    <t xml:space="preserve">
-61°C/1800rpm
-（koolshare,27°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>N/A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1057,12 +925,6 @@
   </si>
   <si>
     <t>www.expreview.com/76107.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS
-AOZ5311QI
-（50A DrMOS）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1077,11 +939,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>73°C/?rpm
-（expreview,27°)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>332
 mm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1103,11 +960,6 @@
   <si>
     <t>6*6mm heat pipes with copper base plate
 metal backplate with thermal pads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>72°C/1940rpm
-（chiphell,21°C)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1116,6 +968,189 @@
 www.expreview.com/76519.html
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colorful iGame GeForce RTX3090 Advanced OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZOTAC GeForce RTX 3080 Apocalypse OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GALAX GeForce RTX 3080 Black General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GALAX GeForce RTX 3080 Metal Master</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9-phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4*8mm heat pipes with copper base plate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVIDIA Geforce RTX3070 Founders Edition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1750MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1725/
+2010MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>220/240W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">8.5cm+8.5cm?
+3800rpm?
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>242
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.techpowerup.com/review/nvidia-geforce-rtx-3070-founders-edition/
+www.expreview.com/76296.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gigabyte GeForce RTX 3070 Gaming OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS AOZ5332QI
+(50A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS
+AOZ5311QI+
+ONSEMI
+NCP303151
+(50A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS
+AOZ5311QI
+(50A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS  
+AOZ5311
+(50A DrMOS)
+OnSemi 
+ON3102
+ON3106</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS  
+AOZ5311
+(50A DrMOS)
+Sinopower SM7342EKKP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1810/
+2010MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70°C/1828rpm
+68°C/2049rpm
+(techpowerup)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">74°C/1791rpm
+(techpowerup)
+76°C/1900rpm
+(expreview,25°C)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.techpowerup.com/review/gigabyte-geforce-rtx-3070-gaming-oc/</t>
+  </si>
+  <si>
+    <t>286
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>115
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>51
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASUS TUF GeForce RTX 3070 Gaming OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnSemi 
+NCP81810</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">63°C/2014rpm
+71°C/1862rpm
+(techpowerup)
+62°C/1900rpm
+66°C/1500rpm
+(chiphell,21°C)
+</t>
+  </si>
+  <si>
+    <t>78°C/1977rpm
+(techpowerup)
+77°C/?rpm
+(expreview,26°C)
+78°C/?rpm
+(pconline)</t>
+  </si>
+  <si>
+    <t>65°C/1807rpm
+70°C/1507rpm
+(expreview,25°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+61°C/1800rpm
+(koolshare,27°C)</t>
   </si>
   <si>
     <t>51°C/3100rpm
@@ -1127,96 +1162,204 @@
 (Turbo BIOS)
 (techpowerup)
 67°C/1725rpm
-（expreview,25°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Colorful iGame GeForce RTX3090 Advanced OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZOTAC GeForce RTX 3080 Apocalypse OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GALAX GeForce RTX 3080 Black General</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GALAX GeForce RTX 3080 Metal Master</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9-phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2-phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS  
-AOZ5311
-Sinopower SM7342EKKP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4*8mm heat pipes with copper base plate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NVIDIA Geforce RTX3070 Founders Edition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1750MHZ</t>
+(expreview,25°C)</t>
+  </si>
+  <si>
+    <t>67°C/2260rpm
+(chiphell,21°C)</t>
+  </si>
+  <si>
+    <t>64°C/2030rpm
+(chiphell,21°C)
+65°C/1838rpm
+76°C/1500rpm
+(techpowerup)</t>
+  </si>
+  <si>
+    <t>72°C/?rpm
+(expreview,25°)</t>
+  </si>
+  <si>
+    <t>73°C/?rpm
+(expreview,27°)</t>
+  </si>
+  <si>
+    <t>72°C/1940rpm
+(chiphell,21°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+71°C/2600rpm
+(expreview,28°C)</t>
+  </si>
+  <si>
+    <t>71°C/1809rpm
+(techpowerup)</t>
+  </si>
+  <si>
+    <t>65°C/1824rpm
+(expreview,27℃)
+65°C/1826rpm
+(3dmgame)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68°C/2175rpm
+68°C/1615rpm
+(techpowerup)
+67°C/1850rpm
+72°C/1500rpm
+(chiphell,21°C)
+</t>
+  </si>
+  <si>
+    <t>68°C/2000?rpm
+(koolshare,27°C)</t>
+  </si>
+  <si>
+    <t>67°C/2016rpm
+77°C/1543rpm
+(techpowerup)</t>
+  </si>
+  <si>
+    <t>76°C/1700rpm
+(techpowerup)</t>
+  </si>
+  <si>
+    <t>74°C/1800rpm
+(expreview,27°C)
+74°C/?rpm
+(pconline)</t>
+  </si>
+  <si>
+    <t>77°C/?rpm
+(pconline)
+73°C/2137rpm
+(3dmgame)</t>
+  </si>
+  <si>
+    <t>65°C/1857rpm
+71°C/1606rpm
+(techpowerup)</t>
+  </si>
+  <si>
+    <t>74°C/?rpm
+(pconline)
+65°C/1953rpm
+(3dmgame,normal)
+65°C/1783rpm
+(3dmgame,Turbo BIOS)</t>
+  </si>
+  <si>
+    <t>AOS AOZ5332QI+
+AOZ5311QI
+(50A DrMOS))</t>
+  </si>
+  <si>
+    <t>AOS AOZ5332QI+
+AOZ5311QI
+(50A DrMOS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1*12PIN
+(only 6 pins are valid)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8PIN+6PIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10-phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>270/270W</t>
+  </si>
+  <si>
+    <t>5*6mm heat pipes with nickel-plated copper base plate
+metal backplate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5*6mm
+heat pipes with direct touching
+metal backplate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1500/
-1725/
+1815/
+1995MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>240/270W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>52mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASUS ROG STRIX GeForce RTX 3070 OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI
+uP9512Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TI NexFET 
+CSD95481RWJ
+(60A DrMOS)
+Onsemi NCP303151</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>280/350W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1905/
 2010MHZ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>220/240W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">8.5cm+8.5cm?
-3800rpm?
+    <t>koolshare.cn/thread-189061-1-1.html
+www.expreview.com/76460.html
+www.chiphell.com/portal.php?mod=view&amp;aid=24447&amp;page=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66°C/1780rpm
+70°C/1380rpm
+(chiphell,20°C)
+63°C/1500rpm
+(expreview,25°C)
+65°C/1700rpm
+(koolshare,27°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">www.techpowerup.com/review/asus-geforce-rtx-3070-tuf-gaming-oc/
+www.chiphell.com/portal.php?mod=view&amp;aid=24447&amp;page=4
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>242
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">74°C/1791rpm
-（techpowerup)
-76°C/1900rpm
-（expreview,25°C)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.techpowerup.com/review/nvidia-geforce-rtx-3070-founders-edition/
-www.expreview.com/76296.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>78°C/1977rpm
-（techpowerup)
-77°C/?rpm
-（expreview,26°C)
-78°C/?rpm
-(pconline)</t>
+    <t>63°C/1768rpm
+(techpowerup)
+61°C/1630rpm
+64°C/13300rpm
+(chiphell,20°C)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1604,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1631,7 +1774,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1640,16 +1783,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -1658,87 +1801,87 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" t="s">
-        <v>32</v>
-      </c>
       <c r="Q1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="57" x14ac:dyDescent="0.2">
@@ -1749,612 +1892,612 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>249</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>21</v>
+        <v>238</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>249</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="R4" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="Q5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="P7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
         <v>57</v>
       </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="O11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R11" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>8</v>
+        <v>249</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="114" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" t="s">
-        <v>151</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -2375,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2402,7 +2545,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2411,16 +2554,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -2429,591 +2572,591 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" t="s">
-        <v>32</v>
-      </c>
       <c r="Q1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="G2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>130</v>
+        <v>232</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>143</v>
+        <v>233</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>248</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -3056,7 +3199,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="R14" s="3"/>
     </row>
@@ -3072,10 +3215,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B74EFA-8FE9-4490-883F-CFD8830FE35D}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R15" sqref="R14:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3101,7 +3244,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3110,16 +3253,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -3128,138 +3271,260 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" t="s">
-        <v>32</v>
-      </c>
       <c r="Q1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C2" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="B5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="G2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="3"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="3"/>
+      <c r="E5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -3284,11 +3549,9 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
+      <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -3300,9 +3563,11 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="3"/>
+      <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -3314,7 +3579,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="2"/>
+      <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F10" s="1"/>
@@ -3356,7 +3621,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="3"/>
+      <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F13" s="1"/>
@@ -3370,7 +3635,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="2"/>
+      <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F14" s="1"/>
@@ -3383,13 +3648,27 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="R14" s="3"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
       <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M16" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add colorful rtx3070 ad
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45334D65-5F01-4C92-9DFC-400E9FEE26BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744EF4ED-BC1D-4C98-AADA-F518547C191E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15975" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="17040" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="255">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -866,22 +866,6 @@
   </si>
   <si>
     <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS  
-AOZ5311
-(50A DrMOS)
-OnSemi 
-ON3102
-ON3106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS  
-AOZ5311
-(50A DrMOS)
-Sinopower SM7342EKKP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1093,13 +1077,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TI NexFET 
-CSD95481RWJ
-(60A DrMOS)
-Onsemi NCP303151</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>280/350W</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1251,6 +1228,78 @@
   </si>
   <si>
     <t>L/W/H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colorful iGame GeForce RTX3070 Advanced OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colorful iGame GeForce RTX3080 Advanced OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TI NexFET 
+CSD95481RWJ
+(60A DrMOS,GPU)
+Onsemi NCP303151
+(Memory)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS  
+AOZ5311
+(50A DrMOS,GPU)
+OnSemi 
+ON3102
+ON3106
+(Memory)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS  
+AOZ5311
+(50A DrMOS,GPU)
+Sinopower SM7342EKKP
+(Memory)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>270/290W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1815/
+1995?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66°C/2258rpm
+(expreview,25°C)
+70°C/2280rpm
+(chiphell,20°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">AOS  
+AOZ5311
+(50A DrMOS,GPU)
+Sinopower
+SM4364A
+SM4373
+(Memory)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>316*131*53
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.chiphell.com/portal.php?mod=view&amp;aid=24447&amp;page=5
+www.expreview.com/76459.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1712,7 +1761,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -1759,10 +1808,10 @@
         <v>79</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -1788,7 +1837,7 @@
         <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -1809,10 +1858,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -1838,7 +1887,7 @@
         <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -1859,10 +1908,10 @@
         <v>128</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -1909,10 +1958,10 @@
         <v>35</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -1962,7 +2011,7 @@
         <v>147</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
@@ -2009,10 +2058,10 @@
         <v>79</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>29</v>
@@ -2059,10 +2108,10 @@
         <v>41</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
@@ -2088,7 +2137,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2109,10 +2158,10 @@
         <v>47</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
@@ -2138,7 +2187,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -2159,10 +2208,10 @@
         <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
@@ -2188,7 +2237,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2209,10 +2258,10 @@
         <v>52</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
@@ -2238,7 +2287,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
@@ -2259,10 +2308,10 @@
         <v>104</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>65</v>
@@ -2309,10 +2358,10 @@
         <v>105</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>65</v>
@@ -2342,7 +2391,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" activeCellId="4" sqref="A1:A1048576 J1:J1048576 L1:L1048576 M1:M1048576 N1:N1048576"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2405,7 +2454,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2452,10 +2501,10 @@
         <v>118</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -2502,10 +2551,10 @@
         <v>129</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2552,10 +2601,10 @@
         <v>81</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -2602,10 +2651,10 @@
         <v>144</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2652,10 +2701,10 @@
         <v>106</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>65</v>
@@ -2666,7 +2715,7 @@
     </row>
     <row r="7" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>245</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -2702,10 +2751,10 @@
         <v>92</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>65</v>
@@ -2752,10 +2801,10 @@
         <v>97</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
@@ -2802,10 +2851,10 @@
         <v>149</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
@@ -2852,10 +2901,10 @@
         <v>150</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
@@ -2881,7 +2930,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2902,10 +2951,10 @@
         <v>92</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
@@ -2969,7 +3018,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3032,7 +3081,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -3041,7 +3090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -3058,10 +3107,10 @@
         <v>163</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>177</v>
+        <v>248</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>164</v>
@@ -3079,10 +3128,10 @@
         <v>168</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -3091,7 +3140,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -3108,45 +3157,45 @@
         <v>175</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>176</v>
+        <v>247</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>130</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s">
         <v>162</v>
@@ -3155,10 +3204,10 @@
         <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -3170,39 +3219,39 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
         <v>162</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E5" t="s">
         <v>175</v>
@@ -3214,45 +3263,82 @@
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>120</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="3"/>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F7" s="1"/>

</xml_diff>

<commit_message>
fix rtx3090 ad error
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744EF4ED-BC1D-4C98-AADA-F518547C191E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF49E2-B23C-4B46-BA16-69ACC3F7D2E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="18105" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -1012,14 +1012,6 @@
 (techpowerup)</t>
   </si>
   <si>
-    <t>74°C/?rpm
-(pconline)
-65°C/1953rpm
-(3dmgame,normal)
-65°C/1783rpm
-(3dmgame,Turbo BIOS)</t>
-  </si>
-  <si>
     <t>AOS AOZ5332QI+
 AOZ5311QI
 (50A DrMOS))</t>
@@ -1300,6 +1292,15 @@
   <si>
     <t>www.chiphell.com/portal.php?mod=view&amp;aid=24447&amp;page=5
 www.expreview.com/76459.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74°C/?rpm
+(pconline)
+65°C/1953rpm
+(3dmgame,normal)
+70°C/1783rpm
+(3dmgame,Turbo BIOS)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1696,9 +1697,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" activeCellId="4" sqref="A1:A1048576 J1:J1048576 L1:L1048576 M1:M1048576 N1:N1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1761,7 +1762,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -1808,10 +1809,10 @@
         <v>79</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -1837,7 +1838,7 @@
         <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -1861,7 +1862,7 @@
         <v>192</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -1887,7 +1888,7 @@
         <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -1911,7 +1912,7 @@
         <v>193</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -1961,7 +1962,7 @@
         <v>194</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2011,7 +2012,7 @@
         <v>147</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
@@ -2061,7 +2062,7 @@
         <v>195</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>29</v>
@@ -2111,7 +2112,7 @@
         <v>196</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
@@ -2137,7 +2138,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2161,7 +2162,7 @@
         <v>197</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
@@ -2187,7 +2188,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -2211,7 +2212,7 @@
         <v>198</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
@@ -2237,7 +2238,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2261,7 +2262,7 @@
         <v>199</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
@@ -2287,7 +2288,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
@@ -2311,7 +2312,7 @@
         <v>200</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>65</v>
@@ -2358,10 +2359,10 @@
         <v>105</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>201</v>
+        <v>254</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>65</v>
@@ -2391,7 +2392,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2454,7 +2455,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2504,7 +2505,7 @@
         <v>183</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -2554,7 +2555,7 @@
         <v>184</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2604,7 +2605,7 @@
         <v>182</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -2654,7 +2655,7 @@
         <v>185</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2704,7 +2705,7 @@
         <v>186</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>65</v>
@@ -2715,7 +2716,7 @@
     </row>
     <row r="7" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -2754,7 +2755,7 @@
         <v>187</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>65</v>
@@ -2804,7 +2805,7 @@
         <v>188</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
@@ -2854,7 +2855,7 @@
         <v>189</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
@@ -2904,7 +2905,7 @@
         <v>190</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
@@ -2930,7 +2931,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2954,7 +2955,7 @@
         <v>191</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
@@ -3016,9 +3017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B74EFA-8FE9-4490-883F-CFD8830FE35D}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3081,7 +3082,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -3107,10 +3108,10 @@
         <v>163</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>164</v>
@@ -3131,7 +3132,7 @@
         <v>178</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -3157,13 +3158,13 @@
         <v>175</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>130</v>
@@ -3175,13 +3176,13 @@
         <v>166</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>177</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -3192,10 +3193,10 @@
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
         <v>162</v>
@@ -3204,10 +3205,10 @@
         <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -3219,25 +3220,25 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
@@ -3245,7 +3246,7 @@
         <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
         <v>162</v>
@@ -3263,39 +3264,39 @@
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>120</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3307,7 +3308,7 @@
         <v>163</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -3319,25 +3320,25 @@
         <v>74</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix tuf rtx3070 pwmic error
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF49E2-B23C-4B46-BA16-69ACC3F7D2E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC02E71B-9011-425F-BC4B-332A1ECBADB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18105" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="19170" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -896,11 +896,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OnSemi 
-NCP81810</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">63°C/2014rpm
 71°C/1862rpm
 (techpowerup)
@@ -1301,6 +1296,11 @@
 (3dmgame,normal)
 70°C/1783rpm
 (3dmgame,Turbo BIOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnSemi 
+NCP81610</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1697,9 +1697,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1762,7 +1762,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -1809,10 +1809,10 @@
         <v>79</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -1838,7 +1838,7 @@
         <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -1859,10 +1859,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -1888,7 +1888,7 @@
         <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -1909,10 +1909,10 @@
         <v>128</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -1959,10 +1959,10 @@
         <v>35</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2012,7 +2012,7 @@
         <v>147</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
@@ -2059,10 +2059,10 @@
         <v>79</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>29</v>
@@ -2109,10 +2109,10 @@
         <v>41</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
@@ -2138,7 +2138,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2159,10 +2159,10 @@
         <v>47</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
@@ -2188,7 +2188,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -2209,10 +2209,10 @@
         <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
@@ -2238,7 +2238,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2259,10 +2259,10 @@
         <v>52</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
@@ -2288,7 +2288,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
@@ -2309,10 +2309,10 @@
         <v>104</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>65</v>
@@ -2359,10 +2359,10 @@
         <v>105</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>65</v>
@@ -2455,7 +2455,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2502,10 +2502,10 @@
         <v>118</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -2552,10 +2552,10 @@
         <v>129</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2602,10 +2602,10 @@
         <v>81</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -2652,10 +2652,10 @@
         <v>144</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2702,10 +2702,10 @@
         <v>106</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>65</v>
@@ -2716,7 +2716,7 @@
     </row>
     <row r="7" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -2752,10 +2752,10 @@
         <v>92</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>65</v>
@@ -2802,10 +2802,10 @@
         <v>97</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
@@ -2852,10 +2852,10 @@
         <v>149</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
@@ -2902,10 +2902,10 @@
         <v>150</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
@@ -2931,7 +2931,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2952,10 +2952,10 @@
         <v>92</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
@@ -3017,9 +3017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B74EFA-8FE9-4490-883F-CFD8830FE35D}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3082,7 +3082,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -3108,10 +3108,10 @@
         <v>163</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>164</v>
@@ -3132,7 +3132,7 @@
         <v>178</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
@@ -3158,13 +3158,13 @@
         <v>175</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>130</v>
@@ -3176,13 +3176,13 @@
         <v>166</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>177</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -3193,10 +3193,10 @@
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
         <v>162</v>
@@ -3205,10 +3205,10 @@
         <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -3220,25 +3220,25 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
@@ -3246,13 +3246,13 @@
         <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
         <v>162</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>181</v>
+        <v>254</v>
       </c>
       <c r="E5" t="s">
         <v>175</v>
@@ -3264,39 +3264,39 @@
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>120</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3308,7 +3308,7 @@
         <v>163</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -3320,25 +3320,25 @@
         <v>74</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>166</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add zotac rtx3070 twin edge oc and x-gaming oc
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7279305-72EC-4A75-BD5F-BFFD00127F05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A8C87B-1CB3-4DD7-8393-540E856EC3E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20235" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="21300" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="280">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1353,6 +1353,75 @@
   </si>
   <si>
     <t>www.techpowerup.com/review/evga-geforce-rtx-3070-ftw3-ultra/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zotac RTX 3070 Twin Edge OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5*6mm heat pipes with nickel-plated copper base plate
+non-metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2*10cm?
+2500rpm?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>220/242W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1755/
+2025MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70°C/1955rpm
+(techpowerup)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.techpowerup.com/review/zotac-geforce-rtx-3070-twin-edge-oc/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>232*141*41.5
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zotac RTX 3070 X-Gaming OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI uP1666Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI uP1666Q?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5*6mm heat pipes with nickel-plated copper base plate
+metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64°C/1720rpm
+(expreview,24°)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>311*118*55
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76455.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1750,8 +1819,8 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2444,7 +2513,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3071,7 +3140,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P17" sqref="P17"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3156,8 +3225,8 @@
       <c r="D2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>163</v>
+      <c r="E2" t="s">
+        <v>275</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>246</v>
@@ -3206,8 +3275,8 @@
       <c r="D3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>175</v>
+      <c r="E3" t="s">
+        <v>275</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>245</v>
@@ -3443,33 +3512,109 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="3"/>
+    <row r="8" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>274</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>

</xml_diff>

<commit_message>
add msi rtx3070 gaming x trio
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A8C87B-1CB3-4DD7-8393-540E856EC3E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C3CD98-D15C-4F08-86B1-EFF5BFF566BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21300" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="22365" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="288">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -473,12 +473,6 @@
   </si>
   <si>
     <t>4-phase6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6*6mm + 1*8mm 
-heat pipes with direct touching
-non-metal backplate with 2 heat pipes and thermal pads(*)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1226,11 +1220,172 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TI NexFET 
-CSD95481RWJ
-(60A DrMOS,GPU)
-Onsemi NCP303151
-(Memory)</t>
+    <t>270/290W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1815/
+1995?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66°C/2258rpm
+(expreview,25°C)
+70°C/2280rpm
+(chiphell,20°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>316*131*53
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.chiphell.com/portal.php?mod=view&amp;aid=24447&amp;page=5
+www.expreview.com/76459.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74°C/?rpm
+(pconline)
+65°C/1953rpm
+(3dmgame,normal)
+70°C/1783rpm
+(3dmgame,Turbo BIOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnSemi 
+NCP81610</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t> EVGA GeForce RTX 3070 FTW3 Ultra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12-phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnSemi 
+NCP81278T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5*8mm? heat pipes with copper base plate
+non-metal backplate with 2 heat pipes and thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*9cm?
+2500rpm?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1815/
+2010MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>270/300W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65°C/1781rpm
+64°C/1940rpm
+(techpowerup)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.techpowerup.com/review/evga-geforce-rtx-3070-ftw3-ultra/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zotac RTX 3070 Twin Edge OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5*6mm heat pipes with nickel-plated copper base plate
+non-metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2*10cm?
+2500rpm?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>220/242W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1755/
+2025MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70°C/1955rpm
+(techpowerup)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.techpowerup.com/review/zotac-geforce-rtx-3070-twin-edge-oc/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>232*141*41.5
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zotac RTX 3070 X-Gaming OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI uP1666Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI uP1666Q?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5*6mm heat pipes with nickel-plated copper base plate
+metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64°C/1720rpm
+(expreview,24°)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>311*118*55
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76455.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.techpowerup.com/review/msi-geforce-rtx-3070-gaming-x-trio/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSI GeForce RTX 3040 Gaming X Trio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS  
+AOZ5311
+(50A DrMOS,GPU)
+Sinopower SM7342EKKP
+(RAM)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1240,32 +1395,15 @@
 OnSemi 
 ON3102
 ON3106
-(Memory)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOS  
-AOZ5311
-(50A DrMOS,GPU)
-Sinopower SM7342EKKP
-(Memory)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>270/290W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1500/
-1815/
-1995?MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>66°C/2258rpm
-(expreview,25°C)
-70°C/2280rpm
-(chiphell,20°C)</t>
+(RAM)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TI NexFET 
+CSD95481RWJ
+(60A DrMOS,GPU)
+Onsemi NCP303151
+(RAM)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1275,45 +1413,8 @@
 Sinopower
 SM4364A
 SM4373
-(Memory)
+(RAM)
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>316*131*53
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.chiphell.com/portal.php?mod=view&amp;aid=24447&amp;page=5
-www.expreview.com/76459.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74°C/?rpm
-(pconline)
-65°C/1953rpm
-(3dmgame,normal)
-70°C/1783rpm
-(3dmgame,Turbo BIOS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnSemi 
-NCP81610</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t> EVGA GeForce RTX 3070 FTW3 Ultra</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12-phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnSemi 
-NCP81278T</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1322,106 +1423,47 @@
 (50A DrMOS,GPU)
 OnSemi 
 FDPC5018SG
-(Memory)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5*8mm? heat pipes with copper base plate
+(RAM)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6*6mm 
+heat pipes with direct touching
+non-metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6*6mm + 1*8mm 
+heat pipes with direct touching
 non-metal backplate with 2 heat pipes and thermal pads</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3*9cm?
-2500rpm?</t>
+    <t>OnSemi 
+NCP302045
+(45A DrMOS,GPU)
+Niko Semi PK616BA
+(RAM)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*9cm
+3400rpm?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1500/
-1815/
-2010MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>270/300W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>65°C/1781rpm
-64°C/1940rpm
+1830/
+2070MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>240/250W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64°C/1510rpm
 (techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.techpowerup.com/review/evga-geforce-rtx-3070-ftw3-ultra/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zotac RTX 3070 Twin Edge OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5*6mm heat pipes with nickel-plated copper base plate
-non-metal backplate with thermal pads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2*10cm?
-2500rpm?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>220/242W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1500/
-1755/
-2025MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>70°C/1955rpm
-(techpowerup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.techpowerup.com/review/zotac-geforce-rtx-3070-twin-edge-oc/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>232*141*41.5
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zotac RTX 3070 X-Gaming OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPI uP1666Q</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPI uP1666Q?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5*6mm heat pipes with nickel-plated copper base plate
-metal backplate with thermal pads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>64°C/1720rpm
-(expreview,24°)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>311*118*55
-mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>www.expreview.com/76455.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1820,7 +1862,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1844,7 +1886,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1853,10 +1895,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
         <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>109</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1883,7 +1925,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -1894,7 +1936,7 @@
     </row>
     <row r="2" spans="1:16" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
         <v>70</v>
@@ -1903,25 +1945,25 @@
         <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>15</v>
@@ -1930,16 +1972,16 @@
         <v>79</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.2">
@@ -1953,13 +1995,13 @@
         <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -1980,10 +2022,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2003,13 +2045,13 @@
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -2027,13 +2069,13 @@
         <v>15</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -2080,10 +2122,10 @@
         <v>35</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2109,7 +2151,7 @@
         <v>72</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>9</v>
@@ -2121,25 +2163,25 @@
         <v>62</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
@@ -2180,10 +2222,10 @@
         <v>79</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>29</v>
@@ -2194,7 +2236,7 @@
     </row>
     <row r="8" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -2206,7 +2248,7 @@
         <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>39</v>
@@ -2215,10 +2257,10 @@
         <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>36</v>
@@ -2230,10 +2272,10 @@
         <v>41</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
@@ -2259,7 +2301,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2280,10 +2322,10 @@
         <v>47</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
@@ -2309,7 +2351,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -2330,10 +2372,10 @@
         <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
@@ -2359,7 +2401,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2380,10 +2422,10 @@
         <v>52</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
@@ -2409,7 +2451,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
@@ -2427,13 +2469,13 @@
         <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>65</v>
@@ -2444,7 +2486,7 @@
     </row>
     <row r="13" spans="1:16" ht="114" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
         <v>70</v>
@@ -2453,13 +2495,13 @@
         <v>95</v>
       </c>
       <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E13" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="G13" t="s">
         <v>26</v>
@@ -2477,13 +2519,13 @@
         <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>65</v>
@@ -2513,7 +2555,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:P8"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2537,7 +2579,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2546,10 +2588,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
         <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>109</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -2576,7 +2618,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2587,60 +2629,60 @@
     </row>
     <row r="2" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
         <v>126</v>
-      </c>
-      <c r="B3" t="s">
-        <v>127</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -2652,7 +2694,7 @@
         <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -2661,33 +2703,33 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>70</v>
@@ -2711,7 +2753,7 @@
         <v>78</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>83</v>
@@ -2723,21 +2765,21 @@
         <v>81</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
@@ -2761,28 +2803,28 @@
         <v>78</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="142.5" x14ac:dyDescent="0.2">
@@ -2802,7 +2844,7 @@
         <v>72</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G6" t="s">
         <v>26</v>
@@ -2820,24 +2862,24 @@
         <v>80</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -2873,10 +2915,10 @@
         <v>92</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>65</v>
@@ -2887,7 +2929,7 @@
     </row>
     <row r="8" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -2899,7 +2941,7 @@
         <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>39</v>
@@ -2908,36 +2950,36 @@
         <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>96</v>
+        <v>282</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
@@ -2952,7 +2994,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2961,33 +3003,33 @@
         <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -3002,42 +3044,42 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -3052,13 +3094,13 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>40</v>
@@ -3073,16 +3115,16 @@
         <v>92</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -3140,7 +3182,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:P10"/>
+      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3164,7 +3206,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3173,10 +3215,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
         <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>109</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -3203,7 +3245,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -3214,60 +3256,60 @@
     </row>
     <row r="2" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
         <v>161</v>
-      </c>
-      <c r="C2" t="s">
-        <v>162</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -3276,60 +3318,60 @@
         <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>244</v>
+        <v>278</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -3341,42 +3383,42 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>39</v>
@@ -3385,39 +3427,39 @@
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3426,10 +3468,10 @@
         <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -3441,190 +3483,226 @@
         <v>74</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s">
         <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
         <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="2"/>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>

</xml_diff>

<commit_message>
add inno3d rtx3070 ichill x4
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C3CD98-D15C-4F08-86B1-EFF5BFF566BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A402D0-11F9-4424-A3C2-9962D719FF2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22365" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="23430" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="2" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="298">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1377,10 +1377,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MSI GeForce RTX 3040 Gaming X Trio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AOS  
 AOZ5311
 (50A DrMOS,GPU)
@@ -1464,6 +1460,68 @@
   <si>
     <t>64°C/1510rpm
 (techpowerup)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSI GeForce RTX 3070 Gaming X Trio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inno3D Geforce RTX3070 Ichill x4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6*6mm
+heat pipes with direct touching
+1*6mm heat pipe for mos
+metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS AOZ5332QI+
+AOZ5311QI
+(50A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS  
+AOZ5311
+(50A DrMOS,GPU)
+UBIQ
+M3816N
+(RAM)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>240/260W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500/
+1785/
+1935?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70°C/1941rpm
+(expreview,26°)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.expreview.com/76560.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300*135
+mm
+"2.5-slot"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*9cm
+?rpm+
+?cm
+?rpm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1861,7 +1919,700 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.625" customWidth="1"/>
+    <col min="2" max="2" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="9.75" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
+    <col min="6" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="14.125" customWidth="1"/>
+    <col min="10" max="10" width="10.625" customWidth="1"/>
+    <col min="11" max="11" width="9.875" customWidth="1"/>
+    <col min="12" max="12" width="10.625" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="11.625" customWidth="1"/>
+    <col min="15" max="15" width="8" customWidth="1"/>
+    <col min="16" max="16" width="62.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="114" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <webPublishItems count="2">
+    <webPublishItem id="28498" divId="GraphicsCardSpecificationTable_28498" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\GraphicsCardSpecificationTable.htm"/>
+    <webPublishItem id="5606" divId="GraphicsCardSpecificationTable_5606" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\Page.html"/>
+  </webPublishItems>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1934,15 +2685,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>136</v>
@@ -1960,48 +2711,48 @@
         <v>115</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.2">
+      <c r="P2" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>139</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -2010,183 +2761,183 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" t="s">
         <v>71</v>
       </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>200</v>
+        <v>85</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>38</v>
+      <c r="D5" t="s">
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
+        <v>85</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="P5" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="E6" t="s">
         <v>72</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
+        <v>172</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -2198,51 +2949,51 @@
         <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>71</v>
@@ -2257,22 +3008,22 @@
         <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>102</v>
+        <v>281</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>100</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>221</v>
@@ -2280,19 +3031,19 @@
       <c r="O8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>42</v>
+      <c r="P8" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
@@ -2301,7 +3052,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2310,39 +3061,39 @@
         <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
@@ -2351,48 +3102,48 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>27</v>
+        <v>151</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="P10" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -2401,161 +3152,95 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P11" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="114" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="P11" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
+      <c r="O14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <webPublishItems count="2">
-    <webPublishItem id="28498" divId="GraphicsCardSpecificationTable_28498" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\GraphicsCardSpecificationTable.htm"/>
-    <webPublishItem id="5606" divId="GraphicsCardSpecificationTable_5606" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\Page.html"/>
-  </webPublishItems>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
-  <dimension ref="A1:P15"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B74EFA-8FE9-4490-883F-CFD8830FE35D}">
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2627,633 +3312,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="57" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>242</v>
-      </c>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B74EFA-8FE9-4490-883F-CFD8830FE35D}">
-  <dimension ref="A1:P16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40.625" customWidth="1"/>
-    <col min="2" max="2" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
-    <col min="5" max="5" width="13.25" customWidth="1"/>
-    <col min="6" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="14.125" customWidth="1"/>
-    <col min="10" max="10" width="10.625" customWidth="1"/>
-    <col min="11" max="11" width="9.875" customWidth="1"/>
-    <col min="12" max="12" width="10.625" customWidth="1"/>
-    <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="11.625" customWidth="1"/>
-    <col min="15" max="15" width="8" customWidth="1"/>
-    <col min="16" max="16" width="62.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="2" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>164</v>
@@ -3271,7 +3329,7 @@
         <v>269</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>201</v>
@@ -3321,7 +3379,7 @@
         <v>269</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>202</v>
@@ -3371,7 +3429,7 @@
         <v>210</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -3471,7 +3529,7 @@
         <v>162</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -3521,7 +3579,7 @@
         <v>252</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -3571,7 +3629,7 @@
         <v>268</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -3621,7 +3679,7 @@
         <v>268</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -3656,7 +3714,7 @@
     </row>
     <row r="10" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="B10" t="s">
         <v>160</v>
@@ -3671,28 +3729,28 @@
         <v>162</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>165</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>221</v>
@@ -3704,17 +3762,55 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="2"/>
+    <row r="11" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s">
+        <v>269</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F12" s="1"/>

</xml_diff>

<commit_message>
add inno3d rtx3080 x4,fix colorful rtx3080 vulcan data error
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFF1D7F-01C2-4FB3-8971-34314044D0A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA749CC2-2B05-444E-800B-20453C88AC44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26625" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="27690" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="321">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -705,10 +705,6 @@
     <t>1440/
 1710/
 1960?MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?/?W</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -910,18 +906,6 @@
 (koolshare,27°C)</t>
   </si>
   <si>
-    <t>51°C/3100rpm
-65°C/1640rpm
-(zol,61°C)
-67°C/1745rpm
-(normal)
-72°C/1912rpm
-(Turbo BIOS)
-(techpowerup)
-67°C/1725rpm
-(expreview,25°C)</t>
-  </si>
-  <si>
     <t>67°C/2260rpm
 (chiphell,21°C)</t>
   </si>
@@ -939,10 +923,6 @@
   <si>
     <t>73°C/?rpm
 (expreview,27°)</t>
-  </si>
-  <si>
-    <t>72°C/1940rpm
-(chiphell,21°C)</t>
   </si>
   <si>
     <t>65°C/1824rpm
@@ -1621,6 +1601,53 @@
   </si>
   <si>
     <t>EVGA GeForce RTX 3090 FTW3 Ultra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diy.pconline.com.cn/1376/13768705.html
+diy.zol.com.cn/753/7537400.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1770/
+2040?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*9cm
+3400rpm+
+?cm
+?rpm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72°C/1940rpm
+(chiphell,21°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>51°C/3100rpm
+65°C/1640rpm
+(zol,25°C)
+67°C/1745rpm
+(normal)
+72°C/1912rpm
+(Turbo BIOS)
+(techpowerup)
+67°C/1725rpm
+(expreview,25°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66°C/1683rpm
+(zol,24°C)
+71°C/?rpm
+(pconline)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inno3D Geforce RTX3080 Ichill x4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2017,9 +2044,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2082,7 +2109,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2129,10 +2156,10 @@
         <v>78</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>64</v>
@@ -2158,7 +2185,7 @@
         <v>70</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -2179,10 +2206,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2208,7 +2235,7 @@
         <v>70</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -2229,10 +2256,10 @@
         <v>125</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -2279,10 +2306,10 @@
         <v>35</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2320,25 +2347,25 @@
         <v>62</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
@@ -2379,10 +2406,10 @@
         <v>78</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>29</v>
@@ -2429,10 +2456,10 @@
         <v>41</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>64</v>
@@ -2458,7 +2485,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2479,10 +2506,10 @@
         <v>47</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>64</v>
@@ -2508,7 +2535,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -2529,10 +2556,10 @@
         <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>64</v>
@@ -2558,7 +2585,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2579,10 +2606,10 @@
         <v>52</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>64</v>
@@ -2593,7 +2620,7 @@
     </row>
     <row r="12" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B12" t="s">
         <v>58</v>
@@ -2608,7 +2635,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
@@ -2629,10 +2656,10 @@
         <v>101</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>64</v>
@@ -2643,7 +2670,7 @@
     </row>
     <row r="13" spans="1:16" ht="114" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s">
         <v>69</v>
@@ -2679,10 +2706,10 @@
         <v>102</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>64</v>
@@ -2710,9 +2737,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2775,7 +2802,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2822,10 +2849,10 @@
         <v>115</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>64</v>
@@ -2851,7 +2878,7 @@
         <v>70</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -2872,10 +2899,10 @@
         <v>126</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2922,16 +2949,16 @@
         <v>80</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
@@ -2969,19 +2996,19 @@
         <v>79</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="142.5" x14ac:dyDescent="0.2">
@@ -3001,7 +3028,7 @@
         <v>71</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" t="s">
         <v>26</v>
@@ -3022,21 +3049,21 @@
         <v>103</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>182</v>
+        <v>318</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B7" t="s">
         <v>69</v>
@@ -3072,10 +3099,10 @@
         <v>91</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>64</v>
@@ -3107,7 +3134,7 @@
         <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>98</v>
@@ -3122,10 +3149,10 @@
         <v>94</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>64</v>
@@ -3136,7 +3163,7 @@
     </row>
     <row r="9" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
@@ -3151,7 +3178,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -3169,13 +3196,13 @@
         <v>79</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>64</v>
@@ -3186,7 +3213,7 @@
     </row>
     <row r="10" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -3201,42 +3228,42 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -3251,13 +3278,13 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>40</v>
@@ -3272,29 +3299,67 @@
         <v>91</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>187</v>
+        <v>317</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="3"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>320</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F13" s="1"/>
@@ -3402,7 +3467,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -3413,60 +3478,60 @@
     </row>
     <row r="2" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
         <v>158</v>
-      </c>
-      <c r="C2" t="s">
-        <v>159</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -3475,60 +3540,60 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>127</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -3540,42 +3605,42 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>39</v>
@@ -3584,39 +3649,39 @@
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>117</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3625,10 +3690,10 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -3640,275 +3705,275 @@
         <v>73</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
         <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D9" t="s">
         <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" t="s">
         <v>158</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="N10" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D11" t="s">
         <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="M11" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -4041,7 +4106,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -4052,102 +4117,102 @@
     </row>
     <row r="2" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add gainward rtx3080 glare oc
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA749CC2-2B05-444E-800B-20453C88AC44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99772EE2-58DF-4545-BECD-1E7364C67595}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27690" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="28755" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="345">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -888,19 +888,6 @@
 </t>
   </si>
   <si>
-    <t>78°C/1977rpm
-(techpowerup)
-77°C/?rpm
-(expreview,26°C)
-78°C/?rpm
-(pconline)</t>
-  </si>
-  <si>
-    <t>65°C/1807rpm
-70°C/1507rpm
-(expreview,25°C)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 61°C/1800rpm
 (koolshare,27°C)</t>
@@ -915,10 +902,6 @@
 65°C/1838rpm
 76°C/1500rpm
 (techpowerup)</t>
-  </si>
-  <si>
-    <t>72°C/?rpm
-(expreview,25°)</t>
   </si>
   <si>
     <t>73°C/?rpm
@@ -957,12 +940,6 @@
 (expreview,27°C)
 74°C/?rpm
 (pconline)</t>
-  </si>
-  <si>
-    <t>77°C/?rpm
-(pconline)
-73°C/2137rpm
-(3dmgame)</t>
   </si>
   <si>
     <t>65°C/1857rpm
@@ -1648,6 +1625,153 @@
   </si>
   <si>
     <t>Inno3D Geforce RTX3080 Ichill x4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASUS ROG STRIX GeForce RTX 3080 OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diy.pconline.com.cn/1379/13794145.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+1905/
+?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>370/450W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Systems
+MP2888A?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI uP9512Q?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TI NexFET 
+CSD95481RWJ?
+(60A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>78°C/1977rpm
+(techpowerup)
+77°C/?rpm
+(expreview,26°C)
+78°C/?rpm
+(pconline)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65°C/1807rpm
+70°C/1507rpm
+(expreview,25°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66°C/?rpm
+(pconline)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inno3D RTX 3080 TWIN X2 OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7*6mm
+heat pipes with direct touching
+metal backplate with thermal pads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2*9cm
+?rpm
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440/
+?/
+?MHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>274*120
+mm
+“3-slot”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.chiphell.com/thread-2278001-1-2.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPI uP9511R?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13-phase?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-phase?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS AOZ5332QI+
+AOZ5311QI?
+(50A DrMOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gainward RTX 3080 Glare OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>329*136*63
+mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOS AOZ5332QI+
+AOZ5311QI
+(50A DrMOS))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*9cm
+2400?rpm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77°C/?rpm
+(pconline)
+73°C/2137rpm
+(3dmgame)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72°C/?rpm
+(expreview,25°)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75°C/?rpm
+(pconline)
+73°C/1815rpm
+(3dmgame)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diy.pconline.com.cn/1371/13715501.html
+3c.3dmgame.com/show-16-13130-1-all.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2044,9 +2168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2109,7 +2233,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2156,10 +2280,10 @@
         <v>78</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>64</v>
@@ -2185,7 +2309,7 @@
         <v>70</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -2206,10 +2330,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2235,7 +2359,7 @@
         <v>70</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -2256,10 +2380,10 @@
         <v>125</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -2306,10 +2430,10 @@
         <v>35</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2359,7 +2483,7 @@
         <v>143</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
@@ -2406,10 +2530,10 @@
         <v>78</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>29</v>
@@ -2456,10 +2580,10 @@
         <v>41</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>64</v>
@@ -2485,7 +2609,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2506,10 +2630,10 @@
         <v>47</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>64</v>
@@ -2535,7 +2659,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -2556,10 +2680,10 @@
         <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>64</v>
@@ -2585,7 +2709,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2606,10 +2730,10 @@
         <v>52</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>191</v>
+        <v>341</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>64</v>
@@ -2620,7 +2744,7 @@
     </row>
     <row r="12" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B12" t="s">
         <v>58</v>
@@ -2635,7 +2759,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
@@ -2656,10 +2780,10 @@
         <v>101</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>64</v>
@@ -2706,10 +2830,10 @@
         <v>102</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>64</v>
@@ -2735,11 +2859,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2802,7 +2926,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2849,10 +2973,10 @@
         <v>115</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>178</v>
+        <v>324</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>64</v>
@@ -2899,10 +3023,10 @@
         <v>126</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>179</v>
+        <v>325</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2911,59 +3035,59 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>317</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
+        <v>143</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>322</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>323</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>82</v>
+        <v>319</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>177</v>
+        <v>326</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>141</v>
+      <c r="P4" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
         <v>69</v>
@@ -2990,142 +3114,142 @@
         <v>117</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="142.5" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
         <v>71</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
+        <v>84</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>318</v>
+        <v>178</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="57" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>236</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>181</v>
+        <v>314</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="P7" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>136</v>
+      <c r="E8" t="s">
+        <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>39</v>
@@ -3134,89 +3258,89 @@
         <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>274</v>
+        <v>66</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="P8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
+      <c r="D9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>168</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>27</v>
+        <v>270</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>132</v>
+      <c r="P9" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3228,42 +3352,42 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>148</v>
+        <v>27</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>184</v>
+        <v>342</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="57" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -3278,42 +3402,42 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>91</v>
+        <v>146</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>317</v>
+        <v>181</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>320</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
@@ -3328,68 +3452,192 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>282</v>
+        <v>189</v>
       </c>
       <c r="G12" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>316</v>
+        <v>40</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>315</v>
+        <v>93</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>79</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="P12" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>327</v>
+      </c>
+      <c r="B14" t="s">
+        <v>334</v>
+      </c>
+      <c r="C14" t="s">
+        <v>335</v>
+      </c>
+      <c r="D14" t="s">
+        <v>333</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="O14" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3467,7 +3715,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -3490,13 +3738,13 @@
         <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>160</v>
@@ -3517,7 +3765,7 @@
         <v>174</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>64</v>
@@ -3540,16 +3788,16 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>127</v>
@@ -3561,13 +3809,13 @@
         <v>162</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>173</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -3578,10 +3826,10 @@
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>158</v>
@@ -3590,10 +3838,10 @@
         <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -3605,25 +3853,25 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
@@ -3631,13 +3879,13 @@
         <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
         <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E5" t="s">
         <v>171</v>
@@ -3649,39 +3897,39 @@
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>117</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3693,7 +3941,7 @@
         <v>159</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -3705,83 +3953,83 @@
         <v>73</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B7" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C7" t="s">
         <v>158</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
         <v>158</v>
@@ -3790,48 +4038,48 @@
         <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
         <v>158</v>
@@ -3840,22 +4088,22 @@
         <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>162</v>
@@ -3864,21 +4112,21 @@
         <v>164</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B10" t="s">
         <v>157</v>
@@ -3887,51 +4135,51 @@
         <v>158</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>159</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C11" t="s">
         <v>158</v>
@@ -3940,40 +4188,40 @@
         <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>64</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -4106,7 +4354,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -4117,102 +4365,102 @@
     </row>
     <row r="2" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>301</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix backplate fan info
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99772EE2-58DF-4545-BECD-1E7364C67595}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E913AC03-7592-4DE7-977B-DBD83D4E7E41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28755" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="29820" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="345">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,13 +287,6 @@
     <t xml:space="preserve">diy.pconline.com.cn/1384/13843225.html
 3c.3dmgame.com/show-16-13190-1-all.html
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3*9cm
-3500rpm+
-?cm
-?rpm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -648,11 +641,6 @@
   </si>
   <si>
     <t>www.expreview.com/76104.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2*9cm+1*8cm
-?rpm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1456,13 +1444,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3*9cm
-?rpm+
-?cm
-?rpm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AMD Radeon RX6800XT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1589,13 +1570,6 @@
     <t>1440/
 1770/
 2040?MHZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3*9cm
-3400rpm+
-?cm
-?rpm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1746,11 +1720,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3*9cm
-2400?rpm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>77°C/?rpm
 (pconline)
 73°C/2137rpm
@@ -1772,6 +1741,35 @@
   <si>
     <t>diy.pconline.com.cn/1371/13715501.html
 3c.3dmgame.com/show-16-13130-1-all.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*9cm
+2400?rpm+
+8cm on backplate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">3*9cm
+3400rpm+
+small fan for mosfet </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">3*9cm
+3500rpm+
+small fan for mosfet </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">3*9cm
+?rpm+
+small fan for mosfet </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2*9cm+1*8cm
+2 fans on backplate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1779,7 +1777,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1800,6 +1798,15 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1825,12 +1832,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1852,9 +1862,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2168,9 +2182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2194,7 +2208,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2203,10 +2217,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" t="s">
-        <v>106</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -2233,7 +2247,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2244,52 +2258,52 @@
     </row>
     <row r="2" spans="1:16" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.2">
@@ -2303,13 +2317,13 @@
         <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -2318,7 +2332,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>32</v>
@@ -2330,10 +2344,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -2353,13 +2367,13 @@
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -2368,7 +2382,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>33</v>
@@ -2377,19 +2391,19 @@
         <v>15</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
@@ -2430,10 +2444,10 @@
         <v>35</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
@@ -2444,107 +2458,107 @@
     </row>
     <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
         <v>70</v>
       </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
         <v>70</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -2553,10 +2567,10 @@
         <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>39</v>
@@ -2565,10 +2579,10 @@
         <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>36</v>
@@ -2580,13 +2594,13 @@
         <v>41</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>42</v>
@@ -2609,7 +2623,7 @@
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2618,7 +2632,7 @@
         <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>48</v>
@@ -2630,15 +2644,15 @@
         <v>47</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" s="7" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2659,7 +2673,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -2680,13 +2694,13 @@
         <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>51</v>
@@ -2709,7 +2723,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -2718,7 +2732,7 @@
         <v>55</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>57</v>
+        <v>342</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>54</v>
@@ -2730,13 +2744,13 @@
         <v>52</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>56</v>
@@ -2744,10 +2758,10 @@
     </row>
     <row r="12" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
@@ -2759,66 +2773,66 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="J12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="114" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="E13" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="G13" t="s">
         <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>33</v>
@@ -2827,19 +2841,19 @@
         <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -2848,8 +2862,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="P9" r:id="rId1" xr:uid="{151F28DC-AB6A-4108-9A07-9A85BF89BD10}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <webPublishItems count="2">
     <webPublishItem id="28498" divId="GraphicsCardSpecificationTable_28498" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\GraphicsCardSpecificationTable.htm"/>
     <webPublishItem id="5606" divId="GraphicsCardSpecificationTable_5606" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\Page.html"/>
@@ -2861,9 +2878,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2887,7 +2904,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2896,10 +2913,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" t="s">
-        <v>106</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -2926,7 +2943,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -2937,72 +2954,72 @@
     </row>
     <row r="2" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
         <v>123</v>
-      </c>
-      <c r="B3" t="s">
-        <v>124</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
@@ -3011,48 +3028,48 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>321</v>
-      </c>
       <c r="E4" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
@@ -3064,192 +3081,192 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
         <v>70</v>
       </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
         <v>70</v>
       </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="K7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>39</v>
@@ -3258,36 +3275,36 @@
         <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -3296,10 +3313,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>39</v>
@@ -3308,39 +3325,39 @@
         <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3352,7 +3369,7 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -3361,33 +3378,33 @@
         <v>27</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -3402,42 +3419,42 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
@@ -3452,42 +3469,42 @@
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G12" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
@@ -3502,7 +3519,7 @@
         <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
@@ -3511,83 +3528,83 @@
         <v>55</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>312</v>
+        <v>341</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>315</v>
-      </c>
       <c r="N13" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B14" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C14" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D14" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E14" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
@@ -3602,7 +3619,7 @@
         <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
@@ -3614,25 +3631,25 @@
         <v>340</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -3652,7 +3669,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3676,7 +3693,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3685,10 +3702,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" t="s">
-        <v>106</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -3715,7 +3732,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -3726,122 +3743,122 @@
     </row>
     <row r="2" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -3853,42 +3870,42 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>39</v>
@@ -3897,331 +3914,331 @@
         <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="M8" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="M9" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="N10" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>285</v>
+        <v>343</v>
       </c>
       <c r="J11" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -4270,7 +4287,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P15" s="3"/>
     </row>
@@ -4315,7 +4332,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4324,10 +4341,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" t="s">
-        <v>106</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -4354,7 +4371,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="O1" t="s">
         <v>28</v>
@@ -4365,102 +4382,102 @@
     </row>
     <row r="2" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -4584,7 +4601,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P13" s="3"/>
     </row>

</xml_diff>

<commit_message>
add fix README error
</commit_message>
<xml_diff>
--- a/GraphicsCardSpecificationSheet.xlsx
+++ b/GraphicsCardSpecificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphicsCardSpecificationSheet\master\GraphicsCardSpecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E913AC03-7592-4DE7-977B-DBD83D4E7E41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EEDB54-C8E5-42B1-AA63-614E5857C0AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29820" yWindow="0" windowWidth="17640" windowHeight="7125" activeTab="1" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
+    <workbookView xWindow="30885" yWindow="0" windowWidth="17640" windowHeight="7125" xr2:uid="{51E77FC5-D503-4A6D-92F4-40DBDE3FABAE}"/>
   </bookViews>
   <sheets>
     <sheet name="RTX3090 24G" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="345">
   <si>
     <t>vGPU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1777,7 +1777,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1798,15 +1798,6 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1832,15 +1823,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1862,13 +1850,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2182,9 +2166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF445520-4C7A-488E-8692-8BF5C6615755}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2652,7 +2636,7 @@
       <c r="O9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="P9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2862,11 +2846,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="P9" r:id="rId1" xr:uid="{151F28DC-AB6A-4108-9A07-9A85BF89BD10}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <webPublishItems count="2">
     <webPublishItem id="28498" divId="GraphicsCardSpecificationTable_28498" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\GraphicsCardSpecificationTable.htm"/>
     <webPublishItem id="5606" divId="GraphicsCardSpecificationTable_5606" sourceType="sheet" destinationFile="D:\GraphicsCardSpecificationTable\Page.html"/>
@@ -2878,9 +2859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932F15D3-D16A-4C3E-9586-404AE588E537}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomLeft" activeCell="N1" activeCellId="4" sqref="A1:A1048576 J1:J1048576 L1:L1048576 M1:M1048576 N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3668,8 +3649,8 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1" activeCellId="4" sqref="A1:A1048576 J1:J1048576 L1:L1048576 M1:M1048576 N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>